<commit_message>
Add Enemy Follow Animated Path
</commit_message>
<xml_diff>
--- a/Assets/Resources/stage01.xlsx
+++ b/Assets/Resources/stage01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\System32\HomeWork\Fourth_First\Unity\KomaGalaga\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C0EA8EF0-FB77-42F0-B246-B37C169E659E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCAED18-735F-46BC-93A3-ECFDE8BE1453}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20880" windowHeight="8385" xr2:uid="{FF8B0DF7-F4C5-4F95-A32B-1E9094834413}"/>
   </bookViews>
@@ -119,7 +119,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -244,13 +244,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -306,6 +343,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -622,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71246E8-7194-4EDF-8889-C4DE19843CAB}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -633,47 +682,53 @@
     <col min="10" max="10" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17.25" thickBot="1">
-      <c r="A1">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
+    <row r="1" spans="1:14" ht="17.25" thickBot="1">
+      <c r="A1" s="19">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20">
+        <v>1</v>
+      </c>
+      <c r="C1" s="20">
+        <v>2</v>
+      </c>
+      <c r="D1" s="20">
         <v>3</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="20">
         <v>4</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="20">
         <v>5</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="20">
         <v>6</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="20">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="I1" s="20">
+        <v>8</v>
+      </c>
+      <c r="J1" s="21">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:14">
       <c r="A2" s="14">
         <v>0</v>
       </c>
-      <c r="B2" s="16">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>3</v>
+      <c r="B2" s="22">
+        <v>0</v>
+      </c>
+      <c r="C2" s="16">
+        <v>0</v>
       </c>
       <c r="D2" s="1">
         <v>3</v>
@@ -684,20 +739,26 @@
       <c r="F2" s="1">
         <v>3</v>
       </c>
-      <c r="G2" s="16">
-        <v>0</v>
-      </c>
-      <c r="H2" s="17">
-        <v>0</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" s="9">
+      <c r="G2" s="1">
+        <v>3</v>
+      </c>
+      <c r="H2" s="22">
+        <v>0</v>
+      </c>
+      <c r="I2" s="22">
+        <v>0</v>
+      </c>
+      <c r="J2" s="17">
+        <v>0</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:14">
       <c r="A3" s="15">
         <v>0</v>
       </c>
@@ -710,7 +771,7 @@
       <c r="D3" s="2">
         <v>2</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="2">
         <v>2</v>
       </c>
       <c r="F3" s="8">
@@ -719,17 +780,23 @@
       <c r="G3" s="8">
         <v>2</v>
       </c>
-      <c r="H3" s="18">
-        <v>0</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" s="4">
+      <c r="H3" s="8">
+        <v>2</v>
+      </c>
+      <c r="I3" s="8">
+        <v>2</v>
+      </c>
+      <c r="J3" s="18">
+        <v>0</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:14">
       <c r="A4" s="15">
         <v>0</v>
       </c>
@@ -742,7 +809,7 @@
       <c r="D4" s="2">
         <v>2</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="2">
         <v>2</v>
       </c>
       <c r="F4" s="8">
@@ -751,17 +818,23 @@
       <c r="G4" s="8">
         <v>2</v>
       </c>
-      <c r="H4" s="18">
-        <v>0</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="4">
+      <c r="H4" s="8">
+        <v>2</v>
+      </c>
+      <c r="I4" s="8">
+        <v>2</v>
+      </c>
+      <c r="J4" s="18">
+        <v>0</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:14">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -771,7 +844,7 @@
       <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="8">
@@ -783,17 +856,23 @@
       <c r="G5" s="8">
         <v>1</v>
       </c>
-      <c r="H5" s="4">
-        <v>1</v>
-      </c>
-      <c r="J5" s="12" t="s">
+      <c r="H5" s="8">
+        <v>1</v>
+      </c>
+      <c r="I5" s="8">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4">
+        <v>1</v>
+      </c>
+      <c r="M5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="4">
+      <c r="N5" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:14">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -803,29 +882,35 @@
       <c r="C6" s="2">
         <v>1</v>
       </c>
-      <c r="D6" s="8">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1</v>
-      </c>
-      <c r="F6" s="8">
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2">
         <v>1</v>
       </c>
       <c r="G6" s="8">
         <v>1</v>
       </c>
-      <c r="H6" s="4">
-        <v>1</v>
-      </c>
-      <c r="J6" s="12" t="s">
+      <c r="H6" s="8">
+        <v>1</v>
+      </c>
+      <c r="I6" s="8">
+        <v>1</v>
+      </c>
+      <c r="J6" s="4">
+        <v>1</v>
+      </c>
+      <c r="M6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="4">
+      <c r="N6" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="17.25" thickBot="1">
+    <row r="7" spans="1:14" ht="17.25" thickBot="1">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -833,35 +918,37 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="7"/>
-      <c r="J7" s="12" t="s">
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="7"/>
+      <c r="M7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="4">
+      <c r="N7" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
-      <c r="J8" s="12" t="s">
+    <row r="8" spans="1:14">
+      <c r="M8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="4">
+      <c r="N8" s="4">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
-      <c r="J9" s="12" t="s">
+    <row r="9" spans="1:14">
+      <c r="M9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K9" s="4">
+      <c r="N9" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="17.25" thickBot="1">
-      <c r="J10" s="13" t="s">
+    <row r="10" spans="1:14" ht="17.25" thickBot="1">
+      <c r="M10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="10">
+      <c r="N10" s="10">
         <v>9</v>
       </c>
     </row>

</xml_diff>